<commit_message>
sprint 4 parte 1
</commit_message>
<xml_diff>
--- a/public/archivos de testing/testing.xlsx
+++ b/public/archivos de testing/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estan\OneDrive\Desktop\Proyecto-final-especializacion\final\public\archivos de testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12C5CB1-C38D-4BCA-B9F5-C3616EF1685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE00F11-0AE0-4494-9D49-EDB3B2D0D514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{455C58AF-73CA-40A4-B411-9CCDEE4845F8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="144">
   <si>
     <t>Id</t>
   </si>
@@ -321,9 +321,6 @@
     <t>deberia verse bien en todos los dispostivos</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Ver importe</t>
   </si>
   <si>
@@ -397,6 +394,84 @@
   </si>
   <si>
     <t>De la lista de tarjetas el usuario debe poder eliminar las tarjetas, si no hay debe mostar un mensaje que no gay tarjetas asociadas</t>
+  </si>
+  <si>
+    <t>Debo poder ingresar dinero de una tarjeta a la cuenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  registrar una tarjeta</t>
+  </si>
+  <si>
+    <t>Ir a cagar dinero</t>
+  </si>
+  <si>
+    <t>Seleccionar tarjeta</t>
+  </si>
+  <si>
+    <t>Elegir monto</t>
+  </si>
+  <si>
+    <t>Al cargar dinero debo ver un cimprobante con el monto agregado y los ultimos 4 digitos de la tarjeta usada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Ingreso de dinero con tarjeta</t>
+  </si>
+  <si>
+    <t>Ingresar dinero de una cuenta externa</t>
+  </si>
+  <si>
+    <t>Debo poder copiar tanto CVU como alias para pasarlo y que me transfieran</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iniciar sesion</t>
+  </si>
+  <si>
+    <t>Ir a cargar dinero</t>
+  </si>
+  <si>
+    <t>ir a tarnsferencia bancaria</t>
+  </si>
+  <si>
+    <t>Debo poder copiar los datos bancarios del usuario o editar el alias</t>
+  </si>
+  <si>
+    <t>Filtro mi actividad</t>
+  </si>
+  <si>
+    <t>Debo poder filtrar mi actividad por fecha (hoy, ayer, etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iniciar sesion </t>
+  </si>
+  <si>
+    <t>clickear en actividad</t>
+  </si>
+  <si>
+    <t>Ir a la lista de actividad</t>
+  </si>
+  <si>
+    <t>clickear filtros y ver</t>
+  </si>
+  <si>
+    <t>Debo poder filtrar por los filtros seleccionados</t>
+  </si>
+  <si>
+    <t>Detalle de la operación</t>
+  </si>
+  <si>
+    <t>Debo poder ver el detalle de la operación al clickear el mismo en la lista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacer una transaccion o deposito </t>
+  </si>
+  <si>
+    <t>clickear una opcion</t>
+  </si>
+  <si>
+    <t>Debo poder ver el detalle de la operación</t>
   </si>
 </sst>
 </file>
@@ -618,7 +693,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="117">
+  <dxfs count="137">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -630,6 +713,158 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
@@ -822,6 +1057,166 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF999999"/>
+          <bgColor rgb="FF999999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF999999"/>
+          <bgColor rgb="FF999999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF999999"/>
+          <bgColor rgb="FF999999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF999999"/>
+          <bgColor rgb="FF999999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFCE5CD"/>
           <bgColor rgb="FFFCE5CD"/>
         </patternFill>
@@ -992,166 +1387,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF93C47D"/>
           <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1865,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328BC580-6FEA-413E-B81F-01462D9B45B6}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:B74"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2857,22 +3092,22 @@
         <v>13</v>
       </c>
       <c r="B51" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="D51" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G51" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="H51" s="14" t="s">
         <v>20</v>
@@ -2893,7 +3128,7 @@
         <v>13</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="15"/>
@@ -2933,22 +3168,22 @@
         <v>14</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H55" s="14" t="s">
         <v>20</v>
@@ -2969,7 +3204,7 @@
         <v>13</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="15"/>
@@ -3009,22 +3244,22 @@
         <v>15</v>
       </c>
       <c r="B59" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="D59" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H59" s="14" t="s">
         <v>20</v>
@@ -3045,7 +3280,7 @@
         <v>13</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="15"/>
@@ -3061,7 +3296,7 @@
         <v>14</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="15"/>
@@ -3087,22 +3322,22 @@
         <v>16</v>
       </c>
       <c r="B63" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="17" t="s">
-        <v>111</v>
-      </c>
       <c r="D63" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H63" s="14" t="s">
         <v>20</v>
@@ -3123,7 +3358,7 @@
         <v>13</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="15"/>
@@ -3139,7 +3374,7 @@
         <v>14</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="15"/>
@@ -3165,22 +3400,22 @@
         <v>17</v>
       </c>
       <c r="B67" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C67" s="17" t="s">
-        <v>116</v>
-      </c>
       <c r="D67" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H67" s="14" t="s">
         <v>20</v>
@@ -3201,7 +3436,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="15"/>
@@ -3217,7 +3452,7 @@
         <v>14</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="15"/>
@@ -3239,24 +3474,36 @@
       <c r="J70" s="16"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
+      <c r="A71" s="14">
+        <v>18</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>118</v>
+      </c>
       <c r="D71" s="17" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="3"/>
-      <c r="G71" s="4"/>
+      <c r="F71" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="H71" s="14" t="s">
         <v>20</v>
       </c>
       <c r="I71" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J71" s="14"/>
+      <c r="J71" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="15"/>
@@ -3266,7 +3513,9 @@
       <c r="E72" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="5"/>
+      <c r="F72" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="G72" s="4"/>
       <c r="H72" s="15"/>
       <c r="I72" s="15"/>
@@ -3280,7 +3529,9 @@
       <c r="E73" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F73" s="5"/>
+      <c r="F73" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="G73" s="6"/>
       <c r="H73" s="15"/>
       <c r="I73" s="15"/>
@@ -3294,56 +3545,484 @@
       <c r="E74" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F74" s="2"/>
+      <c r="F74" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="G74" s="6"/>
       <c r="H74" s="16"/>
       <c r="I74" s="16"/>
       <c r="J74" s="16"/>
     </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="14">
+        <v>19</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I75" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J75" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G76" s="4"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+    </row>
+    <row r="77" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="15"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G77" s="6"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="16"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" s="2"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
+      <c r="J78" s="16"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="14">
+        <v>20</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D79" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I79" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J79" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="15"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G80" s="4"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="15"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G81" s="6"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F82" s="2"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="14">
+        <v>21</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I83" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J83" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="15"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G84" s="4"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="15"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="16"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="14">
+        <v>18</v>
+      </c>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="3"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I87" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J87" s="14"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="15"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F88" s="5"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="15"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="5"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90" s="2"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
+      <c r="J90" s="16"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="14">
+        <v>18</v>
+      </c>
+      <c r="B91" s="17"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" s="3"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I91" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J91" s="14"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="15"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="5"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="15"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="5"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="16"/>
+      <c r="B94" s="16"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" s="2"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="16"/>
+      <c r="J94" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="134">
-    <mergeCell ref="I67:I70"/>
-    <mergeCell ref="J67:J70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="H71:H74"/>
-    <mergeCell ref="I71:I74"/>
-    <mergeCell ref="J71:J74"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="I59:I62"/>
-    <mergeCell ref="J59:J62"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="I63:I66"/>
-    <mergeCell ref="J63:J66"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="H59:H62"/>
-    <mergeCell ref="I51:I54"/>
-    <mergeCell ref="J51:J54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="H55:H58"/>
-    <mergeCell ref="I55:I58"/>
-    <mergeCell ref="J55:J58"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="H51:H54"/>
+  <mergeCells count="169">
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="D91:D94"/>
+    <mergeCell ref="H91:H94"/>
+    <mergeCell ref="I91:I94"/>
+    <mergeCell ref="J91:J94"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="D83:D86"/>
+    <mergeCell ref="H83:H86"/>
+    <mergeCell ref="I83:I86"/>
+    <mergeCell ref="J83:J86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="C87:C90"/>
+    <mergeCell ref="D87:D90"/>
+    <mergeCell ref="H87:H90"/>
+    <mergeCell ref="I87:I90"/>
+    <mergeCell ref="J87:J90"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="H75:H78"/>
+    <mergeCell ref="I75:I78"/>
+    <mergeCell ref="J75:J78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="H79:H82"/>
+    <mergeCell ref="I79:I82"/>
+    <mergeCell ref="J79:J82"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="I47:I50"/>
+    <mergeCell ref="J47:J50"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="I19:I22"/>
+    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="J11:J14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="J3:J6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="I43:I46"/>
     <mergeCell ref="J43:J46"/>
     <mergeCell ref="A43:A46"/>
@@ -3365,443 +4044,514 @@
     <mergeCell ref="C35:C38"/>
     <mergeCell ref="D35:D38"/>
     <mergeCell ref="H35:H38"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="I3:I6"/>
-    <mergeCell ref="J3:J6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="J11:J14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="I19:I22"/>
-    <mergeCell ref="J19:J22"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="J23:J26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="H27:H30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="I23:I26"/>
-    <mergeCell ref="J31:J34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="I47:I50"/>
-    <mergeCell ref="J47:J50"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="I51:I54"/>
+    <mergeCell ref="J51:J54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="H55:H58"/>
+    <mergeCell ref="I55:I58"/>
+    <mergeCell ref="J55:J58"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="J59:J62"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="I63:I66"/>
+    <mergeCell ref="J63:J66"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="H59:H62"/>
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="J67:J70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="H71:H74"/>
+    <mergeCell ref="I71:I74"/>
+    <mergeCell ref="J71:J74"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="H67:H70"/>
   </mergeCells>
   <conditionalFormatting sqref="H3">
+    <cfRule type="cellIs" dxfId="136" priority="89" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="cellIs" dxfId="135" priority="90" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="cellIs" dxfId="134" priority="91" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="cellIs" dxfId="133" priority="92" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="132" priority="85" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="131" priority="86" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="130" priority="87" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="129" priority="88" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="128" priority="81" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="127" priority="82" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="126" priority="83" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="cellIs" dxfId="125" priority="84" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="124" priority="77" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="123" priority="78" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="122" priority="79" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="cellIs" dxfId="121" priority="80" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" dxfId="120" priority="73" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" dxfId="119" priority="74" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" dxfId="118" priority="75" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="cellIs" dxfId="117" priority="76" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
     <cfRule type="cellIs" dxfId="116" priority="69" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="H23">
     <cfRule type="cellIs" dxfId="115" priority="70" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="H23">
     <cfRule type="cellIs" dxfId="114" priority="71" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
+  <conditionalFormatting sqref="H23">
     <cfRule type="cellIs" dxfId="113" priority="72" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="112" priority="65" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="111" priority="66" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="110" priority="67" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H27">
     <cfRule type="cellIs" dxfId="109" priority="68" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H31">
     <cfRule type="cellIs" dxfId="108" priority="61" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H31">
     <cfRule type="cellIs" dxfId="107" priority="62" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H31">
     <cfRule type="cellIs" dxfId="106" priority="63" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H31">
     <cfRule type="cellIs" dxfId="105" priority="64" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="104" priority="57" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="103" priority="58" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="102" priority="59" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="H35">
     <cfRule type="cellIs" dxfId="101" priority="60" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+  <conditionalFormatting sqref="H39">
     <cfRule type="cellIs" dxfId="100" priority="53" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+  <conditionalFormatting sqref="H39">
     <cfRule type="cellIs" dxfId="99" priority="54" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+  <conditionalFormatting sqref="H39">
     <cfRule type="cellIs" dxfId="98" priority="55" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
+  <conditionalFormatting sqref="H39">
     <cfRule type="cellIs" dxfId="97" priority="56" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
+  <conditionalFormatting sqref="H43">
     <cfRule type="cellIs" dxfId="96" priority="49" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
+  <conditionalFormatting sqref="H43">
     <cfRule type="cellIs" dxfId="95" priority="50" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
+  <conditionalFormatting sqref="H43">
     <cfRule type="cellIs" dxfId="94" priority="51" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
+  <conditionalFormatting sqref="H43">
     <cfRule type="cellIs" dxfId="93" priority="52" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="H47">
     <cfRule type="cellIs" dxfId="92" priority="45" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="H47">
     <cfRule type="cellIs" dxfId="91" priority="46" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="H47">
     <cfRule type="cellIs" dxfId="90" priority="47" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="H47">
     <cfRule type="cellIs" dxfId="89" priority="48" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
+  <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="88" priority="41" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
+  <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="87" priority="42" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
+  <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="86" priority="43" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
+  <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="85" priority="44" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H55">
     <cfRule type="cellIs" dxfId="84" priority="37" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H55">
     <cfRule type="cellIs" dxfId="83" priority="38" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H55">
     <cfRule type="cellIs" dxfId="82" priority="39" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+  <conditionalFormatting sqref="H55">
     <cfRule type="cellIs" dxfId="81" priority="40" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H59">
     <cfRule type="cellIs" dxfId="80" priority="33" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H59">
     <cfRule type="cellIs" dxfId="79" priority="34" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H59">
     <cfRule type="cellIs" dxfId="78" priority="35" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H59">
     <cfRule type="cellIs" dxfId="77" priority="36" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H63">
     <cfRule type="cellIs" dxfId="76" priority="29" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H63">
     <cfRule type="cellIs" dxfId="75" priority="30" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H63">
     <cfRule type="cellIs" dxfId="74" priority="31" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="H63">
     <cfRule type="cellIs" dxfId="73" priority="32" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
+  <conditionalFormatting sqref="H67">
     <cfRule type="cellIs" dxfId="72" priority="25" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
+  <conditionalFormatting sqref="H67">
     <cfRule type="cellIs" dxfId="71" priority="26" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
+  <conditionalFormatting sqref="H67">
     <cfRule type="cellIs" dxfId="70" priority="27" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
+  <conditionalFormatting sqref="H67">
     <cfRule type="cellIs" dxfId="69" priority="28" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="48" priority="21" operator="equal">
+  <conditionalFormatting sqref="H71">
+    <cfRule type="cellIs" dxfId="68" priority="21" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="47" priority="22" operator="equal">
+  <conditionalFormatting sqref="H71">
+    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="46" priority="23" operator="equal">
+  <conditionalFormatting sqref="H71">
+    <cfRule type="cellIs" dxfId="66" priority="23" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="45" priority="24" operator="equal">
+  <conditionalFormatting sqref="H71">
+    <cfRule type="cellIs" dxfId="65" priority="24" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="44" priority="17" operator="equal">
+  <conditionalFormatting sqref="H75">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="43" priority="18" operator="equal">
+  <conditionalFormatting sqref="H75">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="42" priority="19" operator="equal">
+  <conditionalFormatting sqref="H75">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="41" priority="20" operator="equal">
+  <conditionalFormatting sqref="H75">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="40" priority="13" operator="equal">
+  <conditionalFormatting sqref="H79">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="39" priority="14" operator="equal">
+  <conditionalFormatting sqref="H79">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="38" priority="15" operator="equal">
+  <conditionalFormatting sqref="H79">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="37" priority="16" operator="equal">
+  <conditionalFormatting sqref="H79">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
+  <conditionalFormatting sqref="H83">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
+  <conditionalFormatting sqref="H83">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
+  <conditionalFormatting sqref="H83">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
+  <conditionalFormatting sqref="H83">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H67">
-    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
+  <conditionalFormatting sqref="H87">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H67">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+  <conditionalFormatting sqref="H87">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H67">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+  <conditionalFormatting sqref="H87">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H67">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+  <conditionalFormatting sqref="H87">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H71">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+  <conditionalFormatting sqref="H91">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H71">
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
+  <conditionalFormatting sqref="H91">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H71">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+  <conditionalFormatting sqref="H91">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H71">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+  <conditionalFormatting sqref="H91">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="J3 J7 J11 J15 J19 J23 J27 J31 J35 J39 J43 J47 J51 J55 J59 J63 J67 J71" xr:uid="{04CF7CF5-A936-4828-AB3D-B5AC4235512F}">
+    <dataValidation type="list" allowBlank="1" sqref="J3 J7 J11 J15 J19 J23 J27 J31 J35 J39 J43 J47 J51 J55 J59 J63 J67 J71 J75 J79 J83 J87 J91" xr:uid="{04CF7CF5-A936-4828-AB3D-B5AC4235512F}">
       <formula1>"Smoke,Regresión"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H3 H7 H11 H15 H19 H23 H27 H31 H35 H39 H43 H47 H51 H55 H59 H63 H67 H71" xr:uid="{6C643EC8-0787-4008-8FB6-C5D7D5716A6E}">
+    <dataValidation type="list" allowBlank="1" sqref="H3 H7 H11 H15 H19 H23 H27 H31 H35 H39 H43 H47 H51 H55 H59 H63 H67 H71 H75 H79 H83 H87 H91" xr:uid="{6C643EC8-0787-4008-8FB6-C5D7D5716A6E}">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4041,177 +4791,177 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C10">
-    <cfRule type="cellIs" dxfId="68" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="31" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C10">
-    <cfRule type="cellIs" dxfId="67" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="32" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C10">
-    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="33" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C10">
-    <cfRule type="cellIs" dxfId="65" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="34" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C10">
-    <cfRule type="cellIs" dxfId="64" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="35" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="27" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="51" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="28" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="50" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="29" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="49" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="30" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="22" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="23" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="24" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="25" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="18" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="19" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="20" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="11" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="12" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="13" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="14" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="15" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4321,52 +5071,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="cellIs" dxfId="63" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="cellIs" dxfId="62" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="cellIs" dxfId="61" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="cellIs" dxfId="60" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C6">
-    <cfRule type="cellIs" dxfId="59" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="57" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="56" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"DEPRECATED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="55" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="54" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>